<commit_message>
Atualização de dados da extração
</commit_message>
<xml_diff>
--- a/_data/in_json/df_artigos_servidores_ingresso_fioce.xlsx
+++ b/_data/in_json/df_artigos_servidores_ingresso_fioce.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FiocruzCeara" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FiocruzCeara" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -30720,12 +30720,12 @@
       </c>
       <c r="K343" t="inlineStr">
         <is>
-          <t>['LEITE-SAMPAIO, N. F.', 'GONDIM, C. N. F. L.', 'MARTINS, R. A. A.', 'SIYADATPANAH, A.', 'NOROUZI, R.', 'KIM, B.', 'SOBRAL-SOUZA, C. E.', 'GONDIM, G. E.', 'RIBEIRO-FILHO, J.', 'COUTINHO, H. D. M. Potentiation of the Activity of Antibiotics against ATCC and MDR Bacterial Strains with (+)-α-Pinene and (-)-Borneol. BIOMED RESEARCH INTERNATIONAL, v. 2022, p. 1-10, 2022.Citações:12|9']</t>
+          <t>['LEITE-SAMPAIO, N. F.', 'GONDIM, C. N. F. L.', 'MARTINS, R. A. A.', 'SIYADATPANAH, A.', 'NOROUZI, R.', 'KIM, B.', 'SOBRAL-SOUZA, C. E.', 'GONDIM, G. E.', 'RIBEIRO-FILHO, J.', 'COUTINHO, H. D. M. Potentiation of the Activity of Antibiotics against ATCC and MDR Bacterial Strains with (+)-α-Pinene and (-)-Borneol. BIOMED RESEARCH INTERNATIONAL, v. 2022, p. 1-10, 2022.Citações:12|13']</t>
         </is>
       </c>
       <c r="L343" t="inlineStr">
         <is>
-          <t>COUTINHO, H. D. M. Potentiation of the Activity of Antibiotics against ATCC and MDR Bacterial Strains with (+)-α-Pinene and (-)-Borneol. BIOMED RESEARCH INTERNATIONAL, v. 2022, p. 1-10, 2022.Citações:12|9</t>
+          <t>COUTINHO, H. D. M. Potentiation of the Activity of Antibiotics against ATCC and MDR Bacterial Strains with (+)-α-Pinene and (-)-Borneol. BIOMED RESEARCH INTERNATIONAL, v. 2022, p. 1-10, 2022.Citações:12|13</t>
         </is>
       </c>
       <c r="M343" t="inlineStr">
@@ -43547,7 +43547,11 @@
       <c r="A489" t="n">
         <v>2023</v>
       </c>
-      <c r="B489" t="inlineStr"/>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>1.9</t>
+        </is>
+      </c>
       <c r="C489" t="inlineStr">
         <is>
           <t>19831447</t>
@@ -53354,7 +53358,11 @@
       <c r="A600" t="n">
         <v>2021</v>
       </c>
-      <c r="B600" t="inlineStr"/>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
       <c r="C600" t="inlineStr">
         <is>
           <t>09717196</t>
@@ -53439,7 +53447,11 @@
       <c r="A601" t="n">
         <v>2020</v>
       </c>
-      <c r="B601" t="inlineStr"/>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
       <c r="C601" t="inlineStr">
         <is>
           <t>22777105</t>
@@ -61243,11 +61255,7 @@
       <c r="A689" t="n">
         <v>2014</v>
       </c>
-      <c r="B689" t="inlineStr">
-        <is>
-          <t>0.534</t>
-        </is>
-      </c>
+      <c r="B689" t="inlineStr"/>
       <c r="C689" t="inlineStr">
         <is>
           <t>01043552</t>
@@ -61332,11 +61340,7 @@
       <c r="A690" t="n">
         <v>2014</v>
       </c>
-      <c r="B690" t="inlineStr">
-        <is>
-          <t>0.534</t>
-        </is>
-      </c>
+      <c r="B690" t="inlineStr"/>
       <c r="C690" t="inlineStr">
         <is>
           <t>15181944</t>

</xml_diff>

<commit_message>
Ajustada extração de preços de medicamentos de alto custo
</commit_message>
<xml_diff>
--- a/_data/in_json/df_artigos_servidores_ingresso_fioce.xlsx
+++ b/_data/in_json/df_artigos_servidores_ingresso_fioce.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FiocruzCeara" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FiocruzCeara" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>